<commit_message>
make a function for reminder
</commit_message>
<xml_diff>
--- a/sample_data/res.xlsx
+++ b/sample_data/res.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="52">
   <si>
     <t>رقم المجموعة</t>
   </si>
@@ -55,9 +55,33 @@
     <t>المجموعة_3</t>
   </si>
   <si>
+    <t>المجموعة_4</t>
+  </si>
+  <si>
+    <t>المجموعة_5</t>
+  </si>
+  <si>
+    <t>المجموعة_6</t>
+  </si>
+  <si>
+    <t>المجموعة_7</t>
+  </si>
+  <si>
+    <t>المجموعة_8</t>
+  </si>
+  <si>
     <t>المجموعة_9</t>
   </si>
   <si>
+    <t>المجموعة_10</t>
+  </si>
+  <si>
+    <t>المجموعة_11</t>
+  </si>
+  <si>
+    <t>المجموعة_12</t>
+  </si>
+  <si>
     <t>أصلية</t>
   </si>
   <si>
@@ -136,7 +160,7 @@
     <t>وفّر عرض ضمن 225-255</t>
   </si>
   <si>
-    <t>مرشح بطول 235 وبعدد ≈ 4</t>
+    <t>مرشح بطول 235 وبعدد ≈ 12</t>
   </si>
   <si>
     <t>مرشح بطول 230 وبعدد ≈ 18</t>
@@ -509,7 +533,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -546,7 +570,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -572,7 +596,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -598,7 +622,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -624,7 +648,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -650,7 +674,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -676,7 +700,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -688,10 +712,10 @@
         <v>300</v>
       </c>
       <c r="F7">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>3300</v>
+        <v>300</v>
       </c>
       <c r="H7">
         <v>12</v>
@@ -702,7 +726,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C8">
         <v>6</v>
@@ -728,25 +752,25 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D9">
-        <v>168</v>
+        <v>200</v>
       </c>
       <c r="E9">
-        <v>235</v>
+        <v>300</v>
       </c>
       <c r="F9">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>1880</v>
+        <v>300</v>
       </c>
       <c r="H9">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -754,53 +778,573 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D10">
-        <v>133</v>
+        <v>200</v>
       </c>
       <c r="E10">
-        <v>190</v>
+        <v>300</v>
       </c>
       <c r="F10">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>2280</v>
+        <v>300</v>
       </c>
       <c r="H10">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>200</v>
+      </c>
+      <c r="E11">
+        <v>300</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>300</v>
+      </c>
+      <c r="H11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>200</v>
+      </c>
+      <c r="E12">
+        <v>300</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>300</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>200</v>
+      </c>
+      <c r="E13">
+        <v>300</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>300</v>
+      </c>
+      <c r="H13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>200</v>
+      </c>
+      <c r="E14">
+        <v>300</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>300</v>
+      </c>
+      <c r="H14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="C11">
-        <f>SUM(C2:C10)</f>
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <f>SUM(D2:D10)</f>
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <f>SUM(E2:E10)</f>
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <f>SUM(F2:F10)</f>
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <f>SUM(G2:G10)</f>
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <f>SUM(H2:H10)</f>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>200</v>
+      </c>
+      <c r="E15">
+        <v>300</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>300</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>200</v>
+      </c>
+      <c r="E16">
+        <v>300</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>300</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>200</v>
+      </c>
+      <c r="E17">
+        <v>300</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>300</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>200</v>
+      </c>
+      <c r="E18">
+        <v>300</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>300</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>133</v>
+      </c>
+      <c r="E19">
+        <v>190</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>190</v>
+      </c>
+      <c r="H19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>133</v>
+      </c>
+      <c r="E20">
+        <v>190</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>190</v>
+      </c>
+      <c r="H20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>133</v>
+      </c>
+      <c r="E21">
+        <v>190</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>190</v>
+      </c>
+      <c r="H21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>133</v>
+      </c>
+      <c r="E22">
+        <v>190</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>190</v>
+      </c>
+      <c r="H22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>133</v>
+      </c>
+      <c r="E23">
+        <v>190</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>190</v>
+      </c>
+      <c r="H23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>133</v>
+      </c>
+      <c r="E24">
+        <v>190</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>190</v>
+      </c>
+      <c r="H24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>133</v>
+      </c>
+      <c r="E25">
+        <v>190</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>190</v>
+      </c>
+      <c r="H25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>133</v>
+      </c>
+      <c r="E26">
+        <v>190</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>190</v>
+      </c>
+      <c r="H26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>133</v>
+      </c>
+      <c r="E27">
+        <v>190</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>190</v>
+      </c>
+      <c r="H27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>133</v>
+      </c>
+      <c r="E28">
+        <v>190</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>190</v>
+      </c>
+      <c r="H28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>133</v>
+      </c>
+      <c r="E29">
+        <v>190</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>190</v>
+      </c>
+      <c r="H29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>133</v>
+      </c>
+      <c r="E30">
+        <v>190</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>190</v>
+      </c>
+      <c r="H30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31">
+        <f>SUM(C2:C30)</f>
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <f>SUM(D2:D30)</f>
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <f>SUM(E2:E30)</f>
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <f>SUM(F2:F30)</f>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f>SUM(G2:G30)</f>
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <f>SUM(H2:H30)</f>
         <v>0</v>
       </c>
     </row>
@@ -811,7 +1355,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -825,16 +1369,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -842,7 +1386,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>378</v>
@@ -862,7 +1406,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>397</v>
@@ -882,16 +1426,16 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>400</v>
       </c>
       <c r="D4">
-        <v>3300</v>
+        <v>300</v>
       </c>
       <c r="E4">
-        <v>720000</v>
+        <v>120000</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -902,16 +1446,16 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C5">
-        <v>301</v>
+        <v>400</v>
       </c>
       <c r="D5">
-        <v>1880</v>
+        <v>300</v>
       </c>
       <c r="E5">
-        <v>619080</v>
+        <v>120000</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -919,22 +1463,182 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>400</v>
+      </c>
+      <c r="D6">
+        <v>300</v>
+      </c>
+      <c r="E6">
+        <v>120000</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>400</v>
+      </c>
+      <c r="D7">
+        <v>300</v>
+      </c>
+      <c r="E7">
+        <v>120000</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="C6">
-        <f>SUM(C2:C5)</f>
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <f>SUM(D2:D5)</f>
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <f>SUM(E2:E5)</f>
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <f>SUM(F2:F5)</f>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>400</v>
+      </c>
+      <c r="D8">
+        <v>300</v>
+      </c>
+      <c r="E8">
+        <v>120000</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>400</v>
+      </c>
+      <c r="D9">
+        <v>300</v>
+      </c>
+      <c r="E9">
+        <v>120000</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>399</v>
+      </c>
+      <c r="D10">
+        <v>190</v>
+      </c>
+      <c r="E10">
+        <v>75810</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>399</v>
+      </c>
+      <c r="D11">
+        <v>190</v>
+      </c>
+      <c r="E11">
+        <v>75810</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12">
+        <v>399</v>
+      </c>
+      <c r="D12">
+        <v>190</v>
+      </c>
+      <c r="E12">
+        <v>75810</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>399</v>
+      </c>
+      <c r="D13">
+        <v>190</v>
+      </c>
+      <c r="E13">
+        <v>75810</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14">
+        <f>SUM(C2:C13)</f>
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <f>SUM(D2:D13)</f>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f>SUM(E2:E13)</f>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f>SUM(F2:F13)</f>
         <v>0</v>
       </c>
     </row>
@@ -953,7 +1657,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -962,10 +1666,10 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1007,7 +1711,7 @@
         <v>235</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1028,7 +1732,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1038,7 +1742,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1046,13 +1750,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -1075,7 +1779,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1092,7 +1796,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1100,7 +1804,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>3300</v>
+        <v>300</v>
       </c>
       <c r="C4">
         <v>400</v>
@@ -1109,7 +1813,7 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1117,29 +1821,165 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>1880</v>
+        <v>300</v>
       </c>
       <c r="C5">
-        <v>301</v>
+        <v>400</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <f>SUM(A2:A5)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <f>SUM(B2:B5)</f>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="C6">
-        <f>SUM(C2:C5)</f>
+        <v>400</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>300</v>
+      </c>
+      <c r="C7">
+        <v>400</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>300</v>
+      </c>
+      <c r="C8">
+        <v>400</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>300</v>
+      </c>
+      <c r="C9">
+        <v>400</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>190</v>
+      </c>
+      <c r="C10">
+        <v>399</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>190</v>
+      </c>
+      <c r="C11">
+        <v>399</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>190</v>
+      </c>
+      <c r="C12">
+        <v>399</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>190</v>
+      </c>
+      <c r="C13">
+        <v>399</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <f>SUM(A2:A13)</f>
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <f>SUM(B2:B13)</f>
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f>SUM(C2:C13)</f>
         <v>0</v>
       </c>
     </row>
@@ -1158,13 +1998,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1172,10 +2012,10 @@
         <v>27152240</v>
       </c>
       <c r="B2">
-        <v>2357320</v>
+        <v>2673160</v>
       </c>
       <c r="C2">
-        <v>24794920</v>
+        <v>24479080</v>
       </c>
     </row>
   </sheetData>
@@ -1193,28 +2033,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1228,16 +2068,16 @@
         <v>235</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="F2">
         <v>168</v>
       </c>
       <c r="H2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1254,13 +2094,13 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F3">
         <v>160</v>
       </c>
       <c r="H3" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1277,13 +2117,13 @@
         <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="F4">
         <v>145</v>
       </c>
       <c r="H4" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1301,7 +2141,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -1316,13 +2156,13 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1348,7 +2188,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1374,7 +2214,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1400,7 +2240,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1426,7 +2266,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1443,16 +2283,16 @@
         <v>182</v>
       </c>
       <c r="E6">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1478,7 +2318,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1504,7 +2344,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:8">

</xml_diff>

<commit_message>
some update on the remainder functions
</commit_message>
<xml_diff>
--- a/sample_data/res.xlsx
+++ b/sample_data/res.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="45">
   <si>
     <t>رقم المجموعة</t>
   </si>
@@ -55,33 +55,9 @@
     <t>المجموعة_3</t>
   </si>
   <si>
-    <t>المجموعة_4</t>
-  </si>
-  <si>
-    <t>المجموعة_5</t>
-  </si>
-  <si>
-    <t>المجموعة_6</t>
-  </si>
-  <si>
-    <t>المجموعة_7</t>
-  </si>
-  <si>
-    <t>المجموعة_8</t>
-  </si>
-  <si>
     <t>المجموعة_9</t>
   </si>
   <si>
-    <t>المجموعة_10</t>
-  </si>
-  <si>
-    <t>المجموعة_11</t>
-  </si>
-  <si>
-    <t>المجموعة_12</t>
-  </si>
-  <si>
     <t>أصلية</t>
   </si>
   <si>
@@ -176,6 +152,9 @@
   </si>
   <si>
     <t>نعم</t>
+  </si>
+  <si>
+    <t>لا</t>
   </si>
 </sst>
 </file>
@@ -533,7 +512,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -570,7 +549,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -596,7 +575,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -622,7 +601,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -648,7 +627,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -674,7 +653,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -700,7 +679,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -712,10 +691,10 @@
         <v>300</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G7">
-        <v>300</v>
+        <v>3600</v>
       </c>
       <c r="H7">
         <v>12</v>
@@ -726,7 +705,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>6</v>
@@ -738,10 +717,10 @@
         <v>300</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G8">
-        <v>300</v>
+        <v>3600</v>
       </c>
       <c r="H8">
         <v>12</v>
@@ -752,25 +731,25 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>200</v>
+        <v>133</v>
       </c>
       <c r="E9">
-        <v>300</v>
+        <v>190</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G9">
-        <v>300</v>
+        <v>2280</v>
       </c>
       <c r="H9">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -778,573 +757,79 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C10">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>200</v>
+        <v>133</v>
       </c>
       <c r="E10">
-        <v>300</v>
+        <v>190</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G10">
-        <v>300</v>
+        <v>2280</v>
       </c>
       <c r="H10">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>200</v>
+        <v>133</v>
       </c>
       <c r="E11">
-        <v>300</v>
+        <v>190</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G11">
-        <v>300</v>
+        <v>2280</v>
       </c>
       <c r="H11">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C12">
-        <v>6</v>
+        <f>SUM(C2:C11)</f>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>200</v>
+        <f>SUM(D2:D11)</f>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>300</v>
+        <f>SUM(E2:E11)</f>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <f>SUM(F2:F11)</f>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>300</v>
+        <f>SUM(G2:G11)</f>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13">
-        <v>6</v>
-      </c>
-      <c r="D13">
-        <v>200</v>
-      </c>
-      <c r="E13">
-        <v>300</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>300</v>
-      </c>
-      <c r="H13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14">
-        <v>6</v>
-      </c>
-      <c r="D14">
-        <v>200</v>
-      </c>
-      <c r="E14">
-        <v>300</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>300</v>
-      </c>
-      <c r="H14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15">
-        <v>6</v>
-      </c>
-      <c r="D15">
-        <v>200</v>
-      </c>
-      <c r="E15">
-        <v>300</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>300</v>
-      </c>
-      <c r="H15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16">
-        <v>6</v>
-      </c>
-      <c r="D16">
-        <v>200</v>
-      </c>
-      <c r="E16">
-        <v>300</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>300</v>
-      </c>
-      <c r="H16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17">
-        <v>6</v>
-      </c>
-      <c r="D17">
-        <v>200</v>
-      </c>
-      <c r="E17">
-        <v>300</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>300</v>
-      </c>
-      <c r="H17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18">
-        <v>6</v>
-      </c>
-      <c r="D18">
-        <v>200</v>
-      </c>
-      <c r="E18">
-        <v>300</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>300</v>
-      </c>
-      <c r="H18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19">
-        <v>133</v>
-      </c>
-      <c r="E19">
-        <v>190</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>190</v>
-      </c>
-      <c r="H19">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20">
-        <v>133</v>
-      </c>
-      <c r="E20">
-        <v>190</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>190</v>
-      </c>
-      <c r="H20">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21">
-        <v>133</v>
-      </c>
-      <c r="E21">
-        <v>190</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>190</v>
-      </c>
-      <c r="H21">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="D22">
-        <v>133</v>
-      </c>
-      <c r="E22">
-        <v>190</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>190</v>
-      </c>
-      <c r="H22">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23">
-        <v>133</v>
-      </c>
-      <c r="E23">
-        <v>190</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23">
-        <v>190</v>
-      </c>
-      <c r="H23">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24">
-        <v>133</v>
-      </c>
-      <c r="E24">
-        <v>190</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24">
-        <v>190</v>
-      </c>
-      <c r="H24">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="D25">
-        <v>133</v>
-      </c>
-      <c r="E25">
-        <v>190</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>190</v>
-      </c>
-      <c r="H25">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26">
-        <v>133</v>
-      </c>
-      <c r="E26">
-        <v>190</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>190</v>
-      </c>
-      <c r="H26">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27">
-        <v>133</v>
-      </c>
-      <c r="E27">
-        <v>190</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>190</v>
-      </c>
-      <c r="H27">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28">
-        <v>133</v>
-      </c>
-      <c r="E28">
-        <v>190</v>
-      </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28">
-        <v>190</v>
-      </c>
-      <c r="H28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29">
-        <v>133</v>
-      </c>
-      <c r="E29">
-        <v>190</v>
-      </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-      <c r="G29">
-        <v>190</v>
-      </c>
-      <c r="H29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30">
-        <v>2</v>
-      </c>
-      <c r="D30">
-        <v>133</v>
-      </c>
-      <c r="E30">
-        <v>190</v>
-      </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="G30">
-        <v>190</v>
-      </c>
-      <c r="H30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31">
-        <f>SUM(C2:C30)</f>
-        <v>0</v>
-      </c>
-      <c r="D31">
-        <f>SUM(D2:D30)</f>
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <f>SUM(E2:E30)</f>
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <f>SUM(F2:F30)</f>
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <f>SUM(G2:G30)</f>
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <f>SUM(H2:H30)</f>
+        <f>SUM(H2:H11)</f>
         <v>0</v>
       </c>
     </row>
@@ -1355,7 +840,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1369,16 +854,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1386,7 +871,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>378</v>
@@ -1406,7 +891,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>397</v>
@@ -1426,16 +911,16 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>400</v>
       </c>
       <c r="D4">
-        <v>300</v>
+        <v>3600</v>
       </c>
       <c r="E4">
-        <v>120000</v>
+        <v>1440000</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -1446,199 +931,39 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C5">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D5">
-        <v>300</v>
+        <v>2280</v>
       </c>
       <c r="E5">
-        <v>120000</v>
+        <v>909720</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>400</v>
+        <f>SUM(C2:C5)</f>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>300</v>
+        <f>SUM(D2:D5)</f>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>120000</v>
+        <f>SUM(E2:E5)</f>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7">
-        <v>400</v>
-      </c>
-      <c r="D7">
-        <v>300</v>
-      </c>
-      <c r="E7">
-        <v>120000</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8">
-        <v>400</v>
-      </c>
-      <c r="D8">
-        <v>300</v>
-      </c>
-      <c r="E8">
-        <v>120000</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9">
-        <v>400</v>
-      </c>
-      <c r="D9">
-        <v>300</v>
-      </c>
-      <c r="E9">
-        <v>120000</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10">
-        <v>399</v>
-      </c>
-      <c r="D10">
-        <v>190</v>
-      </c>
-      <c r="E10">
-        <v>75810</v>
-      </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11">
-        <v>399</v>
-      </c>
-      <c r="D11">
-        <v>190</v>
-      </c>
-      <c r="E11">
-        <v>75810</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12">
-        <v>399</v>
-      </c>
-      <c r="D12">
-        <v>190</v>
-      </c>
-      <c r="E12">
-        <v>75810</v>
-      </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13">
-        <v>399</v>
-      </c>
-      <c r="D13">
-        <v>190</v>
-      </c>
-      <c r="E13">
-        <v>75810</v>
-      </c>
-      <c r="F13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14">
-        <f>SUM(C2:C13)</f>
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <f>SUM(D2:D13)</f>
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <f>SUM(E2:E13)</f>
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <f>SUM(F2:F13)</f>
+        <f>SUM(F2:F5)</f>
         <v>0</v>
       </c>
     </row>
@@ -1657,7 +982,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -1666,10 +991,10 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1732,7 +1057,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1742,7 +1067,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1750,13 +1075,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -1779,7 +1104,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1796,7 +1121,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1804,7 +1129,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>300</v>
+        <v>3600</v>
       </c>
       <c r="C4">
         <v>400</v>
@@ -1813,173 +1138,37 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>300</v>
+        <v>2280</v>
       </c>
       <c r="C5">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>2</v>
+        <f>SUM(A2:A5)</f>
+        <v>0</v>
       </c>
       <c r="B6">
-        <v>300</v>
+        <f>SUM(B2:B5)</f>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>400</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>300</v>
-      </c>
-      <c r="C7">
-        <v>400</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>300</v>
-      </c>
-      <c r="C8">
-        <v>400</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>300</v>
-      </c>
-      <c r="C9">
-        <v>400</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>190</v>
-      </c>
-      <c r="C10">
-        <v>399</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11">
-        <v>3</v>
-      </c>
-      <c r="B11">
-        <v>190</v>
-      </c>
-      <c r="C11">
-        <v>399</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
-        <v>3</v>
-      </c>
-      <c r="B12">
-        <v>190</v>
-      </c>
-      <c r="C12">
-        <v>399</v>
-      </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13">
-        <v>3</v>
-      </c>
-      <c r="B13">
-        <v>190</v>
-      </c>
-      <c r="C13">
-        <v>399</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14">
-        <f>SUM(A2:A13)</f>
-        <v>0</v>
-      </c>
-      <c r="B14">
-        <f>SUM(B2:B13)</f>
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <f>SUM(C2:C13)</f>
+        <f>SUM(C2:C5)</f>
         <v>0</v>
       </c>
     </row>
@@ -1998,13 +1187,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2033,28 +1222,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2071,13 +1260,13 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F2">
         <v>168</v>
       </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2094,13 +1283,13 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F3">
         <v>160</v>
       </c>
       <c r="H3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2117,13 +1306,13 @@
         <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F4">
         <v>145</v>
       </c>
       <c r="H4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2141,7 +1330,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -2156,13 +1345,13 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2188,7 +1377,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2205,16 +1394,16 @@
         <v>12</v>
       </c>
       <c r="E3">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2240,7 +1429,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2266,7 +1455,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2292,7 +1481,7 @@
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2309,16 +1498,16 @@
         <v>12</v>
       </c>
       <c r="E7">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2344,7 +1533,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:8">

</xml_diff>